<commit_message>
Finished community detection algorithm for core myth complex and updated UI to use name attribute
</commit_message>
<xml_diff>
--- a/static/sample/sna/TestDetectionCase.xlsx
+++ b/static/sample/sna/TestDetectionCase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/lucas/ProjectHermes-v2.0/static/sample/sna/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/lucas/GAT/static/sample/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-11380" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="25600" yWindow="-11380" windowWidth="38400" windowHeight="21140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sheet 2017" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -588,6 +588,51 @@
   </si>
   <si>
     <t>Ahmad Khalaf al-Jabouri</t>
+  </si>
+  <si>
+    <t>Sunni Islam</t>
+  </si>
+  <si>
+    <t>Kurdish Nationalism</t>
+  </si>
+  <si>
+    <t>Shiite Islam</t>
+  </si>
+  <si>
+    <t>Neo-Ottomanism</t>
+  </si>
+  <si>
+    <t>Iranian Hegemony</t>
+  </si>
+  <si>
+    <t>BELIMS</t>
+  </si>
+  <si>
+    <t>Iraqi Mosul</t>
+  </si>
+  <si>
+    <t>Pan-Islamism</t>
+  </si>
+  <si>
+    <t>American Hegemony</t>
+  </si>
+  <si>
+    <t>Unified Iraq</t>
+  </si>
+  <si>
+    <t>Unknown Belief</t>
+  </si>
+  <si>
+    <t>Revisionist</t>
+  </si>
+  <si>
+    <t>Ally</t>
+  </si>
+  <si>
+    <t>Defender of the Faith</t>
+  </si>
+  <si>
+    <t>Supporter</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1077,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2745,9 +2790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE215"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4210,73 +4255,133 @@
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="R24" s="13"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="R25" s="13"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="R26" s="13"/>
       <c r="AC26" s="1"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="R30" s="13"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="R31" s="13"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="12"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="R32" s="13"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="R33" s="13"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R34" s="13"/>
       <c r="AC34" s="1"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="R35" s="13"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="R36" s="13"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="R37" s="13"/>
       <c r="AE37" s="1"/>
     </row>

</xml_diff>